<commit_message>
mengubah kriteria dari benefit -> cost
</commit_message>
<xml_diff>
--- a/SAW1.xlsx
+++ b/SAW1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agungperdananto/Documents/SPK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D3B016C-45C0-864C-BB21-4DF3CC85834F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A7C2FEE1-2023-1941-A949-60F0ECD1AD06}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16000" windowHeight="12000" xr2:uid="{CA45C819-B333-9445-AFFD-75815E60935C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{CA45C819-B333-9445-AFFD-75815E60935C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>C1</t>
   </si>
@@ -76,12 +77,18 @@
   </si>
   <si>
     <t xml:space="preserve">A6 = Mira. </t>
+  </si>
+  <si>
+    <t>Hasil Normalisasi Matriks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -117,10 +124,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D83B9CF-A951-DF47-9B4D-1BB78767AB49}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,4 +748,307 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27766107-78A2-1C43-B75A-3A3833586DE4}">
+  <dimension ref="A2:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>70</v>
+      </c>
+      <c r="C4" s="3">
+        <v>50</v>
+      </c>
+      <c r="D4" s="3">
+        <v>80</v>
+      </c>
+      <c r="E4" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>50</v>
+      </c>
+      <c r="C5" s="3">
+        <v>60</v>
+      </c>
+      <c r="D5" s="3">
+        <v>82</v>
+      </c>
+      <c r="E5" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>85</v>
+      </c>
+      <c r="C6" s="3">
+        <v>55</v>
+      </c>
+      <c r="D6" s="3">
+        <v>80</v>
+      </c>
+      <c r="E6" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>82</v>
+      </c>
+      <c r="C7" s="3">
+        <v>70</v>
+      </c>
+      <c r="D7" s="3">
+        <v>65</v>
+      </c>
+      <c r="E7" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <v>75</v>
+      </c>
+      <c r="C8" s="3">
+        <v>75</v>
+      </c>
+      <c r="D8" s="3">
+        <v>85</v>
+      </c>
+      <c r="E8" s="3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3">
+        <v>62</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3">
+        <v>75</v>
+      </c>
+      <c r="E9" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <f>B4/MAX(B4:B9)</f>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="C12" s="3">
+        <f>MIN(C4:C9)/C4</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ref="C12:E12" si="0">D4/MAX(D4:D9)</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="F12" s="3">
+        <f>B12*B2+C12*C2+D12*D2+E12*E2</f>
+        <v>0.87941176470588223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <f>B5/MAX(B4:B9)</f>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="C13" s="3">
+        <f>MIN(C4:C9)/C5</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" ref="C13:E13" si="1">D5/MAX(D4:D9)</f>
+        <v>0.96470588235294119</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="F13" s="3">
+        <f>B13*B2+C13*C2+D13*D2+E13*E2</f>
+        <v>0.77892156862745099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <f>B6/MAX(B4:B9)</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <f>MIN(C4:C9)/C6</f>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" ref="C14:E14" si="2">D6/MAX(D4:D9)</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="F14" s="3">
+        <f>B14*B2+C14*C2+D14*D2+E14*E2</f>
+        <v>0.9449197860962566</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <f>B7/MAX(B4:B9)</f>
+        <v>0.96470588235294119</v>
+      </c>
+      <c r="C15" s="3">
+        <f>MIN(C4:C9)/C7</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" ref="C15:E15" si="3">D7/MAX(D4:D9)</f>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <f>B15*B2+C15*C2+D15*D2+E15*E2</f>
+        <v>0.85739495798319332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <f>B8/MAX(B4:B9)</f>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="C16" s="3">
+        <f>MIN(C4:C9)/C8</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ref="C16:E16" si="4">D8/MAX(D4:D9)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="4"/>
+        <v>0.87058823529411766</v>
+      </c>
+      <c r="F16" s="3">
+        <f>B16*B2+C16*C2+D16*D2+E16*E2</f>
+        <v>0.85607843137254902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <f>B9/MAX(B4:B9)</f>
+        <v>0.72941176470588232</v>
+      </c>
+      <c r="C17" s="3">
+        <f>MIN(C4:C9)/C9</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ref="C17:E17" si="5">D9/MAX(D4:D9)</f>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="5"/>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="F17" s="3">
+        <f>B17*B2+C17*C2+D17*D2+E17*E2</f>
+        <v>0.86705882352941166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add metode weighted product
</commit_message>
<xml_diff>
--- a/SAW1.xlsx
+++ b/SAW1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agungperdananto/Documents/SPK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A7C2FEE1-2023-1941-A949-60F0ECD1AD06}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8A596378-690E-9642-8D5A-1799150034DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{CA45C819-B333-9445-AFFD-75815E60935C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="13520" activeTab="1" xr2:uid="{CA45C819-B333-9445-AFFD-75815E60935C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="19">
   <si>
     <t>C1</t>
   </si>
@@ -80,6 +81,9 @@
   </si>
   <si>
     <t>Hasil Normalisasi Matriks</t>
+  </si>
+  <si>
+    <t>C5</t>
   </si>
 </sst>
 </file>
@@ -87,7 +91,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -98,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +112,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -124,11 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="12" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +464,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E8"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +625,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="C11:E11" si="0">D3/MAX(D3:D8)</f>
+        <f t="shared" ref="D11:E11" si="0">D3/MAX(D3:D8)</f>
         <v>0.94117647058823528</v>
       </c>
       <c r="E11" s="1">
@@ -632,7 +650,7 @@
         <v>0.8</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="C12:E12" si="1">D4/MAX(D3:D8)</f>
+        <f t="shared" ref="D12:E12" si="1">D4/MAX(D3:D8)</f>
         <v>0.96470588235294119</v>
       </c>
       <c r="E12" s="1">
@@ -657,7 +675,7 @@
         <v>0.73333333333333328</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="C13:E13" si="2">D5/MAX(D3:D8)</f>
+        <f t="shared" ref="D13:E13" si="2">D5/MAX(D3:D8)</f>
         <v>0.94117647058823528</v>
       </c>
       <c r="E13" s="1">
@@ -682,7 +700,7 @@
         <v>0.93333333333333335</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="C14:E14" si="3">D6/MAX(D3:D8)</f>
+        <f t="shared" ref="D14:E14" si="3">D6/MAX(D3:D8)</f>
         <v>0.76470588235294112</v>
       </c>
       <c r="E14" s="1">
@@ -751,10 +769,256 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2167D0E-C940-1E43-8988-0E37B89EE786}">
+  <dimension ref="A2:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>500</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>350</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <f>MIN(B4:B7)/B4</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <f>C4/MAX(C4:C7)</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <f>D4/MAX(D4:D7)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E11" s="1">
+        <f>MIN(E4:E7)/E4</f>
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="1">
+        <f>F4/MAX(F4:F7)</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <f>B11*B2+C11*C2+D11*D2+E11*E2+F11*F2</f>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
+        <f>MIN(B4:B7)/B5</f>
+        <v>0.3</v>
+      </c>
+      <c r="C12" s="1">
+        <f>C5/MAX(C4:C7)</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <f>D5/MAX(D4:D7)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E12" s="1">
+        <f>MIN(E4:E7)/E5</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F12" s="1">
+        <f>F5/MAX(F4:F7)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G12" s="1">
+        <f>B12*B2+C12*C2+D12*D2+E12*E2+F12*F2</f>
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5">
+        <f>MIN(B4:B7)/B6</f>
+        <v>0.75</v>
+      </c>
+      <c r="C13" s="5">
+        <f>C6/MAX(C4:C7)</f>
+        <v>0.05</v>
+      </c>
+      <c r="D13" s="5">
+        <f>D6/MAX(D4:D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <f>MIN(E4:E7)/E6</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
+        <f>F6/MAX(F4:F7)</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <f>B13*B2+C13*C2+D13*D2+E13*E2+F13*F2</f>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
+        <f>MIN(B4:B7)/B7</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="C14" s="1">
+        <f>C7/MAX(C4:C7)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="1">
+        <f>D7/MAX(D4:D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <f>MIN(E4:E7)/E7</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <f>F7/MAX(F4:F7)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G14" s="1">
+        <f>B14*B2+C14*C2+D14*D2+E14*E2+F14*F2</f>
+        <v>0.73571428571428565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27766107-78A2-1C43-B75A-3A3833586DE4}">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="109" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -911,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" ref="C12:E12" si="0">D4/MAX(D4:D9)</f>
+        <f t="shared" ref="D12:E12" si="0">D4/MAX(D4:D9)</f>
         <v>0.94117647058823528</v>
       </c>
       <c r="E12" s="3">
@@ -936,7 +1200,7 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ref="C13:E13" si="1">D5/MAX(D4:D9)</f>
+        <f t="shared" ref="D13:E13" si="1">D5/MAX(D4:D9)</f>
         <v>0.96470588235294119</v>
       </c>
       <c r="E13" s="3">
@@ -961,7 +1225,7 @@
         <v>0.90909090909090906</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" ref="C14:E14" si="2">D6/MAX(D4:D9)</f>
+        <f t="shared" ref="D14:E14" si="2">D6/MAX(D4:D9)</f>
         <v>0.94117647058823528</v>
       </c>
       <c r="E14" s="3">
@@ -986,7 +1250,7 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" ref="C15:E15" si="3">D7/MAX(D4:D9)</f>
+        <f t="shared" ref="D15:E15" si="3">D7/MAX(D4:D9)</f>
         <v>0.76470588235294112</v>
       </c>
       <c r="E15" s="3">
@@ -1011,7 +1275,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" ref="C16:E16" si="4">D8/MAX(D4:D9)</f>
+        <f t="shared" ref="D16:E16" si="4">D8/MAX(D4:D9)</f>
         <v>1</v>
       </c>
       <c r="E16" s="3">
@@ -1036,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" ref="C17:E17" si="5">D9/MAX(D4:D9)</f>
+        <f t="shared" ref="D17:E17" si="5">D9/MAX(D4:D9)</f>
         <v>0.88235294117647056</v>
       </c>
       <c r="E17" s="3">

</xml_diff>

<commit_message>
tambah ppt weighted product
</commit_message>
<xml_diff>
--- a/SAW1.xlsx
+++ b/SAW1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agungperdananto/Documents/SPK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8A596378-690E-9642-8D5A-1799150034DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A63AF791-2BC2-7249-9BA2-1564E0D12449}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="13520" activeTab="1" xr2:uid="{CA45C819-B333-9445-AFFD-75815E60935C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{CA45C819-B333-9445-AFFD-75815E60935C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -102,18 +102,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -123,7 +117,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39994506668294322"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -143,10 +137,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="12" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="12" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D83B9CF-A951-DF47-9B4D-1BB78767AB49}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -486,10 +480,6 @@
       <c r="E1" s="1">
         <v>0.15</v>
       </c>
-      <c r="F1" s="1">
-        <f>SUM(B1:E1)</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -621,11 +611,11 @@
         <v>0.82352941176470584</v>
       </c>
       <c r="C11" s="1">
-        <f>C3/MAX(C3:C8)</f>
+        <f t="shared" ref="C11:E11" si="0">C3/MAX(C3:C8)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:E11" si="0">D3/MAX(D3:D8)</f>
+        <f t="shared" si="0"/>
         <v>0.94117647058823528</v>
       </c>
       <c r="E11" s="1">
@@ -646,11 +636,11 @@
         <v>0.58823529411764708</v>
       </c>
       <c r="C12" s="1">
-        <f>C4/MAX(C3:C8)</f>
+        <f t="shared" ref="C12:E12" si="1">C4/MAX(C3:C8)</f>
         <v>0.8</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="D12:E12" si="1">D4/MAX(D3:D8)</f>
+        <f t="shared" si="1"/>
         <v>0.96470588235294119</v>
       </c>
       <c r="E12" s="1">
@@ -671,11 +661,11 @@
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <f>C5/MAX(C3:C8)</f>
+        <f t="shared" ref="C13:E13" si="2">C5/MAX(C3:C8)</f>
         <v>0.73333333333333328</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="D13:E13" si="2">D5/MAX(D3:D8)</f>
+        <f t="shared" si="2"/>
         <v>0.94117647058823528</v>
       </c>
       <c r="E13" s="1">
@@ -696,11 +686,11 @@
         <v>0.96470588235294119</v>
       </c>
       <c r="C14" s="1">
-        <f>C6/MAX(C3:C8)</f>
+        <f t="shared" ref="C14:E14" si="3">C6/MAX(C3:C8)</f>
         <v>0.93333333333333335</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:E14" si="3">D6/MAX(D3:D8)</f>
+        <f t="shared" si="3"/>
         <v>0.76470588235294112</v>
       </c>
       <c r="E14" s="1">
@@ -713,26 +703,26 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="4">
         <f>B7/MAX(B3:B8)</f>
         <v>0.88235294117647056</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <f t="shared" ref="C15:E15" si="4">C7/MAX(C3:C8)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="4">
         <f t="shared" si="4"/>
         <v>0.87058823529411766</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="4">
         <f>B15*B1+C15*C1+D15*D1+E15*E1</f>
         <v>0.93941176470588239</v>
       </c>
@@ -769,11 +759,314 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27766107-78A2-1C43-B75A-3A3833586DE4}">
+  <dimension ref="A2:F17"/>
+  <sheetViews>
+    <sheetView zoomScale="109" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>70</v>
+      </c>
+      <c r="C4" s="2">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2">
+        <v>80</v>
+      </c>
+      <c r="E4" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2">
+        <v>82</v>
+      </c>
+      <c r="E5" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>85</v>
+      </c>
+      <c r="C6" s="2">
+        <v>55</v>
+      </c>
+      <c r="D6" s="2">
+        <v>80</v>
+      </c>
+      <c r="E6" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2">
+        <v>70</v>
+      </c>
+      <c r="D7" s="2">
+        <v>65</v>
+      </c>
+      <c r="E7" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>75</v>
+      </c>
+      <c r="C8" s="2">
+        <v>75</v>
+      </c>
+      <c r="D8" s="2">
+        <v>85</v>
+      </c>
+      <c r="E8" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <f>B4/MAX(B4:B9)</f>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="C12" s="2">
+        <f>MIN(C4:C9)/C4</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" ref="D12:E12" si="0">D4/MAX(D4:D9)</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="F12" s="2">
+        <f>B12*B2+C12*C2+D12*D2+E12*E2</f>
+        <v>0.87941176470588223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <f>B5/MAX(B4:B9)</f>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="C13" s="2">
+        <f>MIN(C4:C9)/C5</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" ref="D13:E13" si="1">D5/MAX(D4:D9)</f>
+        <v>0.96470588235294119</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="F13" s="2">
+        <f>B13*B2+C13*C2+D13*D2+E13*E2</f>
+        <v>0.77892156862745099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <f>B6/MAX(B4:B9)</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <f>MIN(C4:C9)/C6</f>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" ref="D14:E14" si="2">D6/MAX(D4:D9)</f>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="F14" s="2">
+        <f>B14*B2+C14*C2+D14*D2+E14*E2</f>
+        <v>0.9449197860962566</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <f>B7/MAX(B4:B9)</f>
+        <v>0.96470588235294119</v>
+      </c>
+      <c r="C15" s="2">
+        <f>MIN(C4:C9)/C7</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" ref="D15:E15" si="3">D7/MAX(D4:D9)</f>
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <f>B15*B2+C15*C2+D15*D2+E15*E2</f>
+        <v>0.85739495798319332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <f>B8/MAX(B4:B9)</f>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="C16" s="2">
+        <f>MIN(C4:C9)/C8</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" ref="D16:E16" si="4">D8/MAX(D4:D9)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="4"/>
+        <v>0.87058823529411766</v>
+      </c>
+      <c r="F16" s="2">
+        <f>B16*B2+C16*C2+D16*D2+E16*E2</f>
+        <v>0.85607843137254902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <f>B9/MAX(B4:B9)</f>
+        <v>0.72941176470588232</v>
+      </c>
+      <c r="C17" s="2">
+        <f>MIN(C4:C9)/C9</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" ref="D17:E17" si="5">D9/MAX(D4:D9)</f>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="5"/>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="F17" s="2">
+        <f>B17*B2+C17*C2+D17*D2+E17*E2</f>
+        <v>0.86705882352941166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2167D0E-C940-1E43-8988-0E37B89EE786}">
   <dimension ref="A2:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="176" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,7 +1089,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -805,7 +1098,7 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
@@ -816,7 +1109,7 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>150</v>
       </c>
       <c r="C4">
@@ -825,7 +1118,7 @@
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>2</v>
       </c>
       <c r="F4">
@@ -836,7 +1129,7 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>500</v>
       </c>
       <c r="C5">
@@ -845,7 +1138,7 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>3</v>
       </c>
       <c r="F5">
@@ -856,7 +1149,7 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>200</v>
       </c>
       <c r="C6">
@@ -865,7 +1158,7 @@
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>1</v>
       </c>
       <c r="F6">
@@ -876,7 +1169,7 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>350</v>
       </c>
       <c r="C7">
@@ -885,7 +1178,7 @@
       <c r="D7">
         <v>3</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>1</v>
       </c>
       <c r="F7">
@@ -954,27 +1247,27 @@
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <f>MIN(B4:B7)/B6</f>
         <v>0.75</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <f>C6/MAX(C4:C7)</f>
         <v>0.05</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <f>D6/MAX(D4:D7)</f>
         <v>1</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f>MIN(E4:E7)/E6</f>
         <v>1</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f>F6/MAX(F4:F7)</f>
         <v>1</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f>B13*B2+C13*C2+D13*D2+E13*E2+F13*F2</f>
         <v>0.76</v>
       </c>
@@ -1012,307 +1305,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27766107-78A2-1C43-B75A-3A3833586DE4}">
-  <dimension ref="A2:F17"/>
-  <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="6" width="10.83203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>70</v>
-      </c>
-      <c r="C4" s="3">
-        <v>50</v>
-      </c>
-      <c r="D4" s="3">
-        <v>80</v>
-      </c>
-      <c r="E4" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3">
-        <v>50</v>
-      </c>
-      <c r="C5" s="3">
-        <v>60</v>
-      </c>
-      <c r="D5" s="3">
-        <v>82</v>
-      </c>
-      <c r="E5" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>85</v>
-      </c>
-      <c r="C6" s="3">
-        <v>55</v>
-      </c>
-      <c r="D6" s="3">
-        <v>80</v>
-      </c>
-      <c r="E6" s="3">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3">
-        <v>82</v>
-      </c>
-      <c r="C7" s="3">
-        <v>70</v>
-      </c>
-      <c r="D7" s="3">
-        <v>65</v>
-      </c>
-      <c r="E7" s="3">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3">
-        <v>75</v>
-      </c>
-      <c r="C8" s="3">
-        <v>75</v>
-      </c>
-      <c r="D8" s="3">
-        <v>85</v>
-      </c>
-      <c r="E8" s="3">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3">
-        <v>62</v>
-      </c>
-      <c r="C9" s="3">
-        <v>50</v>
-      </c>
-      <c r="D9" s="3">
-        <v>75</v>
-      </c>
-      <c r="E9" s="3">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3">
-        <f>B4/MAX(B4:B9)</f>
-        <v>0.82352941176470584</v>
-      </c>
-      <c r="C12" s="3">
-        <f>MIN(C4:C9)/C4</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" ref="D12:E12" si="0">D4/MAX(D4:D9)</f>
-        <v>0.94117647058823528</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>0.70588235294117652</v>
-      </c>
-      <c r="F12" s="3">
-        <f>B12*B2+C12*C2+D12*D2+E12*E2</f>
-        <v>0.87941176470588223</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3">
-        <f>B5/MAX(B4:B9)</f>
-        <v>0.58823529411764708</v>
-      </c>
-      <c r="C13" s="3">
-        <f>MIN(C4:C9)/C5</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" ref="D13:E13" si="1">D5/MAX(D4:D9)</f>
-        <v>0.96470588235294119</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="1"/>
-        <v>0.82352941176470584</v>
-      </c>
-      <c r="F13" s="3">
-        <f>B13*B2+C13*C2+D13*D2+E13*E2</f>
-        <v>0.77892156862745099</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3">
-        <f>B6/MAX(B4:B9)</f>
-        <v>1</v>
-      </c>
-      <c r="C14" s="3">
-        <f>MIN(C4:C9)/C6</f>
-        <v>0.90909090909090906</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" ref="D14:E14" si="2">D6/MAX(D4:D9)</f>
-        <v>0.94117647058823528</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="2"/>
-        <v>0.88235294117647056</v>
-      </c>
-      <c r="F14" s="3">
-        <f>B14*B2+C14*C2+D14*D2+E14*E2</f>
-        <v>0.9449197860962566</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3">
-        <f>B7/MAX(B4:B9)</f>
-        <v>0.96470588235294119</v>
-      </c>
-      <c r="C15" s="3">
-        <f>MIN(C4:C9)/C7</f>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" ref="D15:E15" si="3">D7/MAX(D4:D9)</f>
-        <v>0.76470588235294112</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="F15" s="3">
-        <f>B15*B2+C15*C2+D15*D2+E15*E2</f>
-        <v>0.85739495798319332</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3">
-        <f>B8/MAX(B4:B9)</f>
-        <v>0.88235294117647056</v>
-      </c>
-      <c r="C16" s="3">
-        <f>MIN(C4:C9)/C8</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" ref="D16:E16" si="4">D8/MAX(D4:D9)</f>
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="4"/>
-        <v>0.87058823529411766</v>
-      </c>
-      <c r="F16" s="3">
-        <f>B16*B2+C16*C2+D16*D2+E16*E2</f>
-        <v>0.85607843137254902</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3">
-        <f>B9/MAX(B4:B9)</f>
-        <v>0.72941176470588232</v>
-      </c>
-      <c r="C17" s="3">
-        <f>MIN(C4:C9)/C9</f>
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" ref="D17:E17" si="5">D9/MAX(D4:D9)</f>
-        <v>0.88235294117647056</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" si="5"/>
-        <v>0.94117647058823528</v>
-      </c>
-      <c r="F17" s="3">
-        <f>B17*B2+C17*C2+D17*D2+E17*E2</f>
-        <v>0.86705882352941166</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>